<commit_message>
user symmetric for popularity and asymmetric for rating in overlap similiraty with mean recommender + graph excel
</commit_message>
<xml_diff>
--- a/case-based/readme/case-based-graph.xlsx
+++ b/case-based/readme/case-based-graph.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task1" sheetId="1" r:id="rId1"/>
+    <sheet name="Task2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>topN</t>
   </si>
@@ -57,6 +58,27 @@
   </si>
   <si>
     <t>Precision for jaccardCaseSimilarity | MeanRecommender</t>
+  </si>
+  <si>
+    <t>overlapCaseSimilarity | MaxRecommender | movie popularity symmetric sim</t>
+  </si>
+  <si>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | movie popularity symmetric sim</t>
+  </si>
+  <si>
+    <t>overlapCaseSimilarity | MaxRecommender | movie mean rating asymmetric sim</t>
+  </si>
+  <si>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | movie mean rating asymmetric sim</t>
+  </si>
+  <si>
+    <t>overlapCaseSimilarity | MaxRecommender | movie popularity symmetric sim | movie mean rating asymmetric sim</t>
+  </si>
+  <si>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | movie popularity symmetric sim | movie mean rating asymmetric sim</t>
+  </si>
+  <si>
+    <t>….</t>
   </si>
 </sst>
 </file>
@@ -527,7 +549,7 @@
                   <c:v>0.01295</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0133599999999999</c:v>
+                  <c:v>0.0113599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0129666666666666</c:v>
@@ -985,7 +1007,858 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Precision =</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> f(Recall)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task2!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | movie popularity symmetric sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task2!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.151902617423504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.277184690183807</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.383722615015072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.442470091323048</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.457344459097099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.468336634159447</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.483055150424298</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.493580923952057</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.503076273433212</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.512864113712295</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task2!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.196199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.176699999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.137899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11536</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0999000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0890857142857149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0807</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0736444444444453</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0682600000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task2!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | movie mean rating asymmetric sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task2!$B$17:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0300168269096741</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0709779618669029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0868395196174432</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10131969413668</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.115473713310632</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.129291611405293</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.141419833615627</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.148981501405073</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.158752391029435</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.168196687811964</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task2!$C$17:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0510000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0572000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0477333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0410999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0376799999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0349666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0306999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0291999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0278999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task2!$C$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | movie popularity symmetric sim | movie mean rating asymmetric sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task2!$B$30:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.157156232656503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.286424690081958</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.396614232087169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.456133170146378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.472216477978526</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48657673149202</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.499672574615904</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.510479015123178</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.522097508110112</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.533231973223972</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task2!$C$30:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.203199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.183199999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.165866666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.142049999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11924</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.103566666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0923142857142863</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.083375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0764222222222231</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0709800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task2!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>….</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task2!$B$43:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task2!$C$43:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2139432496"/>
+        <c:axId val="-2117250976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2139432496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Recall</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2117250976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2117250976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Pr</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>écision</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2139432496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1541,6 +2414,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1560,6 +2949,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="10" name="Graphique 9"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1841,8 +3267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2194,7 +3620,7 @@
         <v>4.0431348371323297E-2</v>
       </c>
       <c r="C34">
-        <v>1.33599999999999E-2</v>
+        <v>1.13599999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2381,6 +3807,448 @@
       </c>
       <c r="C52">
         <v>2.0019999999999798E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.151902617423504</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.19619999999999899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.27718469018380698</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.176699999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.38372261501507199</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.16020000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.44247009132304799</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.137899999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.45734445909709898</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.11536</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.46833663415944699</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.9900000000000294E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.48305515042429797</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8.9085714285714906E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.49358092395205699</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8.0699999999999994E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0.50307627343321204</v>
+      </c>
+      <c r="C12">
+        <v>7.3644444444445303E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>0.51286411371229501</v>
+      </c>
+      <c r="C13">
+        <v>6.8260000000000098E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3.00168269096741E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5.1000000000000101E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.0977961866902903E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5.7200000000000299E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.6839519617443198E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.77333333333336E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.10131969413668</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.1099999999999901E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.115473713310632</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.7679999999999603E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.12929161140529299</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3.4966666666666903E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.14141983361562699</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.2999999999999897E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.14898150140507299</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3.06999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>0.158752391029435</v>
+      </c>
+      <c r="C25">
+        <v>2.91999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>0.16819668781196401</v>
+      </c>
+      <c r="C26">
+        <v>2.7899999999999599E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>0.157156232656503</v>
+      </c>
+      <c r="C30">
+        <v>0.20319999999999899</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>0.28642469008195798</v>
+      </c>
+      <c r="C31">
+        <v>0.183199999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>0.39661423208716901</v>
+      </c>
+      <c r="C32">
+        <v>0.165866666666667</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>0.456133170146378</v>
+      </c>
+      <c r="C33">
+        <v>0.14204999999999901</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>0.47221647797852601</v>
+      </c>
+      <c r="C34">
+        <v>0.11924</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.48657673149202002</v>
+      </c>
+      <c r="C35">
+        <v>0.103566666666666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0.49967257461590397</v>
+      </c>
+      <c r="C36">
+        <v>9.2314285714286307E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>0.51047901512317795</v>
+      </c>
+      <c r="C37">
+        <v>8.3375000000000005E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>0.52209750811011202</v>
+      </c>
+      <c r="C38">
+        <v>7.6422222222223099E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>0.53323197322397198</v>
+      </c>
+      <c r="C39">
+        <v>7.0980000000000099E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compute weight dynamically, all is ready to code * RecommenderPersonalised & RecommenderNonPersonalised extends Recommender * Execute utils factorized * CaseSimilarity with dynamic weight
</commit_message>
<xml_diff>
--- a/case-based/readme/case-based-graph.xlsx
+++ b/case-based/readme/case-based-graph.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Task1" sheetId="1" r:id="rId1"/>
     <sheet name="Task2 - 1 " sheetId="2" r:id="rId2"/>
     <sheet name="Task2 - 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Task3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
   <si>
     <t>topN</t>
   </si>
@@ -101,6 +102,12 @@
   </si>
   <si>
     <t>Precision for overlapCaseSimilarity | MaxRecommender | movie popularity symmetric | movie mean rating asymmetric higher value</t>
+  </si>
+  <si>
+    <t>overlapCaseSimilarity | MaxRecommender | task3</t>
+  </si>
+  <si>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | task3</t>
   </si>
 </sst>
 </file>
@@ -719,11 +726,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2136522976"/>
-        <c:axId val="-2136516544"/>
+        <c:axId val="-2140707808"/>
+        <c:axId val="-2140701376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2136522976"/>
+        <c:axId val="-2140707808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,12 +829,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136516544"/>
+        <c:crossAx val="-2140701376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2136516544"/>
+        <c:axId val="-2140701376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +952,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136522976"/>
+        <c:crossAx val="-2140707808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1671,7 +1678,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1679,11 +1685,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2101874336"/>
-        <c:axId val="-2101645696"/>
+        <c:axId val="-2140554144"/>
+        <c:axId val="-2140533232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2101874336"/>
+        <c:axId val="-2140554144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,12 +1763,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101645696"/>
+        <c:crossAx val="-2140533232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2101645696"/>
+        <c:axId val="-2140533232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1850,7 +1856,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101874336"/>
+        <c:crossAx val="-2140554144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2492,11 +2498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103432704"/>
-        <c:axId val="-2105038928"/>
+        <c:axId val="-2140605520"/>
+        <c:axId val="-2140587744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103432704"/>
+        <c:axId val="-2140605520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2595,12 +2601,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105038928"/>
+        <c:crossAx val="-2140587744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105038928"/>
+        <c:axId val="-2140587744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2718,7 +2724,818 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103432704"/>
+        <c:crossAx val="-2140605520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Precision =</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> f(Recall)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0203802135823745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0569020595329529</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0843981835557637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.100845723534888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.113159897522775</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.126741910253064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.138489929150107</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.146503288305435</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.156359230799434</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.164044569093654</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0464000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0457333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0405499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0364399999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0341666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0321142857142856</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0286444444444443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0272599999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | task3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$17:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0192532245186898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0505539758529117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0889931416224544</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.104721150987931</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.121951280064216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13752745231872</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.149166292449461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.155528736573003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.163697814419755</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17081058326205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$17:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0375999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0411000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0465333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0417999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0386799999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0361333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0334857142857142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0307999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0290222222222221</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0274199999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | task3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$30:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0192532245186898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0505539758529117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0889931416224544</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.104721150987931</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.121951280064216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13752745231872</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.149166292449461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.155528736573003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.163697814419755</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17081058326205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$30:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0375999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0411000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0465333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0417999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0386799999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0361333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0334857142857142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0307999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0290222222222221</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0274199999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for jaccardCaseSimilarity | MeanRecommender</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$43:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$43:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2115581824"/>
+        <c:axId val="-2117210576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2115581824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Recall</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2117210576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2117210576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Pr</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>écision</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2115581824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2922,6 +3739,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3955,6 +4812,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4556,6 +5929,43 @@
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4845,7 +6255,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C39"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5396,7 +6806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B55" sqref="B55:C65"/>
     </sheetView>
   </sheetViews>
@@ -6080,7 +7490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="E3" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -6626,4 +8036,496 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.0380213582374501E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.6902059532952902E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6400000000000198E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.4398183555763701E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.5733333333333598E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.10084572353488799</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.0549999999999899E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.113159897522775</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.6439999999999598E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.126741910253064</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.4166666666666901E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.13848992915010699</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.2114285714285602E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.14650328830543499</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9999999999999801E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0.15635923079943401</v>
+      </c>
+      <c r="C12">
+        <v>2.8644444444444299E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>0.164044569093654</v>
+      </c>
+      <c r="C13">
+        <v>2.7259999999999701E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.9253224518689799E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3.7599999999999897E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5.0553975852911701E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4.1100000000000199E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.8993141622454405E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.65333333333336E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.104721150987931</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.17999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.121951280064216</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.86799999999995E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.13752745231871999</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3.61333333333336E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.149166292449461</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.3485714285714202E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.15552873657300301</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3.07999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>0.16369781441975501</v>
+      </c>
+      <c r="C25">
+        <v>2.9022222222222099E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>0.17081058326205001</v>
+      </c>
+      <c r="C26">
+        <v>2.7419999999999601E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>1.9253224518689799E-2</v>
+      </c>
+      <c r="C30">
+        <v>3.7599999999999897E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>5.0553975852911701E-2</v>
+      </c>
+      <c r="C31">
+        <v>4.1100000000000199E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>8.8993141622454405E-2</v>
+      </c>
+      <c r="C32">
+        <v>4.65333333333336E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>0.104721150987931</v>
+      </c>
+      <c r="C33">
+        <v>4.17999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>0.121951280064216</v>
+      </c>
+      <c r="C34">
+        <v>3.86799999999995E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.13752745231871999</v>
+      </c>
+      <c r="C35">
+        <v>3.61333333333336E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0.149166292449461</v>
+      </c>
+      <c r="C36">
+        <v>3.3485714285714202E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>0.15552873657300301</v>
+      </c>
+      <c r="C37">
+        <v>3.07999999999998E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>0.16369781441975501</v>
+      </c>
+      <c r="C38">
+        <v>2.9022222222222099E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>0.17081058326205001</v>
+      </c>
+      <c r="C39">
+        <v>2.7419999999999601E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
success task 3 ! dynamic weight for directors and genres + static weight for artist
</commit_message>
<xml_diff>
--- a/case-based/readme/case-based-graph.xlsx
+++ b/case-based/readme/case-based-graph.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Task1" sheetId="1" r:id="rId1"/>
-    <sheet name="Task2 - 1 " sheetId="2" r:id="rId2"/>
-    <sheet name="Task2 - 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Task3" sheetId="4" r:id="rId4"/>
+    <sheet name="Task3" sheetId="4" r:id="rId1"/>
+    <sheet name="Task1" sheetId="1" r:id="rId2"/>
+    <sheet name="Task2 - 1 " sheetId="2" r:id="rId3"/>
+    <sheet name="Task2 - 2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>topN</t>
   </si>
@@ -104,10 +104,22 @@
     <t>Precision for overlapCaseSimilarity | MaxRecommender | movie popularity symmetric | movie mean rating asymmetric higher value</t>
   </si>
   <si>
-    <t>overlapCaseSimilarity | MaxRecommender | task3</t>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | static directors = 1 only</t>
   </si>
   <si>
-    <t>Precision for overlapCaseSimilarity | MaxRecommender | task3</t>
+    <t>overlapCaseSimilarity | MaxRecommender | static directors = static genres = 1 only</t>
+  </si>
+  <si>
+    <t>overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres only</t>
+  </si>
+  <si>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres only</t>
+  </si>
+  <si>
+    <t>overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres &amp; static actors = 1</t>
+  </si>
+  <si>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres &amp; static actors = 1</t>
   </si>
 </sst>
 </file>
@@ -166,6 +178,877 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Precision =</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> f(Recall)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0203802135823745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0569020595329529</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0843981835557637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.100845723534888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.113159897522775</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.126741910253064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.138489929150107</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.146503288305435</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.156359230799434</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.164044569093654</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0464000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0457333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0405499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0364399999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0341666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0321142857142856</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0286444444444443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0272599999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | static directors = 1 only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$17:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.015483433355763</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0462378293223519</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0675235882747287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0835311775348166</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0977179551471877</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.113770434172071</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.127737352559784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.137758668853834</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.145142610734127</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.150197096990673</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$17:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0227999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0345000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0347333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0326500000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0309599999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0301333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0290571428571427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0277499999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.026511111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0250799999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$30:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0204061253993961</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0512606270999039</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0705514406226962</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0845181160231516</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.100697499706794</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1182932421922</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.137503102112429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.157450649420373</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.175422995320265</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.191261384593387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$30:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0317999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0403000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0372666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0338000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0325199999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0313333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0308571428571427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0303749999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0301333333333332</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0294799999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Task3!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres &amp; static actors = 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Task3!$B$43:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0204792199688122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0602276980956696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0859343779444504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.100058126508605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.113695873915949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.128931231749876</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.141056377419401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.155378233962289</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16645955855214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.175956980684102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Task3!$C$43:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0490000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0469333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0408999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0369599999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0348666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.032742857142857</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0313999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.029911111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0285799999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2115581824"/>
+        <c:axId val="-2117210576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2115581824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Recall</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2117210576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2117210576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Pr</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>écision</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2115581824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1036,7 +1919,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1937,7 +2820,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2808,817 +3691,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Precision =</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> f(Recall)</a:t>
-            </a:r>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Task3!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Task3!$B$4:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0203802135823745</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0569020595329529</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0843981835557637</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.100845723534888</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.113159897522775</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.126741910253064</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.138489929150107</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.146503288305435</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.156359230799434</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.164044569093654</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Task3!$C$4:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0398</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0464000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0457333333333336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0405499999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0364399999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0341666666666669</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0321142857142856</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0299999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0286444444444443</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0272599999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Task3!$C$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | task3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Task3!$B$17:$B$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0192532245186898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0505539758529117</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0889931416224544</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.104721150987931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.121951280064216</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.13752745231872</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.149166292449461</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.155528736573003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.163697814419755</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.17081058326205</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Task3!$C$17:$C$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0375999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0411000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0465333333333336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0417999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0386799999999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0361333333333336</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0334857142857142</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0307999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0290222222222221</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0274199999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Task3!$C$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | task3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Task3!$B$30:$B$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0192532245186898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0505539758529117</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0889931416224544</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.104721150987931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.121951280064216</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.13752745231872</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.149166292449461</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.155528736573003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.163697814419755</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.17081058326205</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Task3!$C$30:$C$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0375999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0411000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0465333333333336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0417999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0386799999999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0361333333333336</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0334857142857142</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0307999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0290222222222221</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0274199999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Task3!$C$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Precision for jaccardCaseSimilarity | MeanRecommender</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Task3!$B$43:$B$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Task3!$C$43:$C$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2115581824"/>
-        <c:axId val="-2117210576"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="-2115581824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="fr-FR"/>
-                  <a:t>Recall</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2117210576"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="-2117210576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="fr-FR"/>
-                  <a:t>Pr</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>écision</a:t>
-                </a:r>
-                <a:endParaRPr lang="fr-FR"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2115581824"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5860,6 +5932,43 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="10" name="Graphique 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
@@ -5878,7 +5987,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5915,7 +6024,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5929,43 +6038,6 @@
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6254,6 +6326,558 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:C52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.0380213582374501E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.6902059532952902E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6400000000000198E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.4398183555763701E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.5733333333333598E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.10084572353488799</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.0549999999999899E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.113159897522775</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.6439999999999598E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.126741910253064</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.4166666666666901E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.13848992915010699</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.2114285714285602E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.14650328830543499</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9999999999999801E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0.15635923079943401</v>
+      </c>
+      <c r="C12">
+        <v>2.8644444444444299E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>0.164044569093654</v>
+      </c>
+      <c r="C13">
+        <v>2.7259999999999701E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.5483433355763E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.27999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4.6237829322351903E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.45000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6.7523588274728694E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.4733333333333297E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.3531177534816606E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.26500000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9.7717955147187702E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.0959999999999599E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.113770434172071</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3.0133333333333599E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.127737352559784</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2.9057142857142702E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.137758668853834</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.7749999999999799E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>0.14514261073412699</v>
+      </c>
+      <c r="C25">
+        <v>2.6511111111110999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>0.15019709699067299</v>
+      </c>
+      <c r="C26">
+        <v>2.50799999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>2.04061253993961E-2</v>
+      </c>
+      <c r="C30">
+        <v>3.1799999999999898E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>5.1260627099903901E-2</v>
+      </c>
+      <c r="C31">
+        <v>4.0300000000000197E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>7.0551440622696193E-2</v>
+      </c>
+      <c r="C32">
+        <v>3.7266666666666698E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>8.4518116023151596E-2</v>
+      </c>
+      <c r="C33">
+        <v>3.3800000000000101E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>0.10069749970679399</v>
+      </c>
+      <c r="C34">
+        <v>3.2519999999999598E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.1182932421922</v>
+      </c>
+      <c r="C35">
+        <v>3.1333333333333602E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0.137503102112429</v>
+      </c>
+      <c r="C36">
+        <v>3.0857142857142701E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>0.15745064942037301</v>
+      </c>
+      <c r="C37">
+        <v>3.0374999999999801E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>0.17542299532026501</v>
+      </c>
+      <c r="C38">
+        <v>3.01333333333332E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>0.19126138459338701</v>
+      </c>
+      <c r="C39">
+        <v>2.94799999999996E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>2.04792199688122E-2</v>
+      </c>
+      <c r="C43">
+        <v>3.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>6.02276980956696E-2</v>
+      </c>
+      <c r="C44">
+        <v>4.90000000000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>8.5934377944450399E-2</v>
+      </c>
+      <c r="C45">
+        <v>4.6933333333333598E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>0.100058126508605</v>
+      </c>
+      <c r="C46">
+        <v>4.0899999999999902E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>0.113695873915949</v>
+      </c>
+      <c r="C47">
+        <v>3.6959999999999597E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>30</v>
+      </c>
+      <c r="B48">
+        <v>0.128931231749876</v>
+      </c>
+      <c r="C48">
+        <v>3.48666666666669E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>35</v>
+      </c>
+      <c r="B49">
+        <v>0.141056377419401</v>
+      </c>
+      <c r="C49">
+        <v>3.2742857142856997E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>40</v>
+      </c>
+      <c r="B50">
+        <v>0.155378233962289</v>
+      </c>
+      <c r="C50">
+        <v>3.1399999999999803E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>45</v>
+      </c>
+      <c r="B51">
+        <v>0.16645955855214001</v>
+      </c>
+      <c r="C51">
+        <v>2.9911111111111E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>0.17595698068410201</v>
+      </c>
+      <c r="C52">
+        <v>2.8579999999999599E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C52"/>
+  <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
@@ -6802,7 +7426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
@@ -7486,7 +8110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
@@ -8036,496 +8660,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.0380213582374501E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.9800000000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5.6902059532952902E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4.6400000000000198E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1">
-        <v>8.4398183555763701E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4.5733333333333598E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.10084572353488799</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4.0549999999999899E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.113159897522775</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3.6439999999999598E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.126741910253064</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3.4166666666666901E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>35</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.13848992915010699</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3.2114285714285602E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>40</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.14650328830543499</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.9999999999999801E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>45</v>
-      </c>
-      <c r="B12">
-        <v>0.15635923079943401</v>
-      </c>
-      <c r="C12">
-        <v>2.8644444444444299E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>0.164044569093654</v>
-      </c>
-      <c r="C13">
-        <v>2.7259999999999701E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.9253224518689799E-2</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3.7599999999999897E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1">
-        <v>5.0553975852911701E-2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>4.1100000000000199E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1">
-        <v>8.8993141622454405E-2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>4.65333333333336E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.104721150987931</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4.17999999999999E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>25</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.121951280064216</v>
-      </c>
-      <c r="C21" s="1">
-        <v>3.86799999999995E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.13752745231871999</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3.61333333333336E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>35</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.149166292449461</v>
-      </c>
-      <c r="C23" s="1">
-        <v>3.3485714285714202E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>40</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.15552873657300301</v>
-      </c>
-      <c r="C24" s="1">
-        <v>3.07999999999998E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>45</v>
-      </c>
-      <c r="B25">
-        <v>0.16369781441975501</v>
-      </c>
-      <c r="C25">
-        <v>2.9022222222222099E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>50</v>
-      </c>
-      <c r="B26">
-        <v>0.17081058326205001</v>
-      </c>
-      <c r="C26">
-        <v>2.7419999999999601E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>5</v>
-      </c>
-      <c r="B30">
-        <v>1.9253224518689799E-2</v>
-      </c>
-      <c r="C30">
-        <v>3.7599999999999897E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>10</v>
-      </c>
-      <c r="B31">
-        <v>5.0553975852911701E-2</v>
-      </c>
-      <c r="C31">
-        <v>4.1100000000000199E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>15</v>
-      </c>
-      <c r="B32">
-        <v>8.8993141622454405E-2</v>
-      </c>
-      <c r="C32">
-        <v>4.65333333333336E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>20</v>
-      </c>
-      <c r="B33">
-        <v>0.104721150987931</v>
-      </c>
-      <c r="C33">
-        <v>4.17999999999999E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>25</v>
-      </c>
-      <c r="B34">
-        <v>0.121951280064216</v>
-      </c>
-      <c r="C34">
-        <v>3.86799999999995E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>30</v>
-      </c>
-      <c r="B35">
-        <v>0.13752745231871999</v>
-      </c>
-      <c r="C35">
-        <v>3.61333333333336E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>0.149166292449461</v>
-      </c>
-      <c r="C36">
-        <v>3.3485714285714202E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>40</v>
-      </c>
-      <c r="B37">
-        <v>0.15552873657300301</v>
-      </c>
-      <c r="C37">
-        <v>3.07999999999998E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>45</v>
-      </c>
-      <c r="B38">
-        <v>0.16369781441975501</v>
-      </c>
-      <c r="C38">
-        <v>2.9022222222222099E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>50</v>
-      </c>
-      <c r="B39">
-        <v>0.17081058326205001</v>
-      </c>
-      <c r="C39">
-        <v>2.7419999999999601E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
shitty as well with no negative weight
</commit_message>
<xml_diff>
--- a/case-based/readme/case-based-graph.xlsx
+++ b/case-based/readme/case-based-graph.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Task3" sheetId="4" r:id="rId1"/>
-    <sheet name="Task1" sheetId="1" r:id="rId2"/>
-    <sheet name="Task2 - 1 " sheetId="2" r:id="rId3"/>
-    <sheet name="Task2 - 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Task3 - 2" sheetId="5" r:id="rId2"/>
+    <sheet name="Task1" sheetId="1" r:id="rId3"/>
+    <sheet name="Task2 - 1 " sheetId="2" r:id="rId4"/>
+    <sheet name="Task2 - 2" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="36">
   <si>
     <t>topN</t>
   </si>
@@ -120,6 +121,21 @@
   </si>
   <si>
     <t>Precision for overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres &amp; static actors = 1</t>
+  </si>
+  <si>
+    <t>››</t>
+  </si>
+  <si>
+    <t>genre distinc between movie case</t>
+  </si>
+  <si>
+    <t>genre distinct beetween user ratings</t>
+  </si>
+  <si>
+    <t>Precision for overlapCaseSimilarity | MaxRecommender | w directors = w actors = w genres = 1</t>
+  </si>
+  <si>
+    <t>overlapCaseSimilarity | MaxRecommender | 'static w directors  w genres = 1 only'</t>
   </si>
 </sst>
 </file>
@@ -267,7 +283,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender</c:v>
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | w directors = w actors = w genres = 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -539,34 +555,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0204061253993961</c:v>
+                  <c:v>0.00626608126341098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0512606270999039</c:v>
+                  <c:v>0.0140316382911608</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0705514406226962</c:v>
+                  <c:v>0.0194949970560057</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0845181160231516</c:v>
+                  <c:v>0.0229944515415114</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.100697499706794</c:v>
+                  <c:v>0.0282282253594312</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1182932421922</c:v>
+                  <c:v>0.031705702120497</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.137503102112429</c:v>
+                  <c:v>0.0341864219845113</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.157450649420373</c:v>
+                  <c:v>0.0381707438688271</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.175422995320265</c:v>
+                  <c:v>0.0440661629329273</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.191261384593387</c:v>
+                  <c:v>0.0463245087121253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,34 +594,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0317999999999999</c:v>
+                  <c:v>0.0119999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0403000000000002</c:v>
+                  <c:v>0.0144999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0372666666666667</c:v>
+                  <c:v>0.0141999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0338000000000001</c:v>
+                  <c:v>0.0129</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0325199999999996</c:v>
+                  <c:v>0.0125599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0313333333333336</c:v>
+                  <c:v>0.0120333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0308571428571427</c:v>
+                  <c:v>0.0113428571428571</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0303749999999998</c:v>
+                  <c:v>0.011025</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0301333333333332</c:v>
+                  <c:v>0.0111555555555555</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0294799999999996</c:v>
+                  <c:v>0.0105799999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -656,36 +672,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0204792199688122</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0602276980956696</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0859343779444504</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.100058126508605</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.113695873915949</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.128931231749876</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.141056377419401</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.155378233962289</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.16645955855214</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.175956980684102</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -695,36 +681,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0398</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0490000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0469333333333336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0408999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0369599999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0348666666666669</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.032742857142857</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0313999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.029911111111111</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0285799999999996</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1134,6 +1090,877 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'Task3 - 2'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0203802135823745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0569020595329529</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0843981835557637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.100845723534888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.113159897522775</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.126741910253064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.138489929150107</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.146503288305435</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.156359230799434</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.164044569093654</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0464000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0457333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0405499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0364399999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0341666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0321142857142856</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0286444444444443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0272599999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task3 - 2'!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | static directors = 1 only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$B$17:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.015483433355763</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0462378293223519</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0675235882747287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0835311775348166</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0977179551471877</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.113770434172071</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.127737352559784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.137758668853834</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.145142610734127</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.150197096990673</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$C$17:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0227999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0345000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0347333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0326500000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0309599999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0301333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0290571428571427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0277499999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.026511111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0250799999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task3 - 2'!$C$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$B$30:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0204061253993961</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0512606270999039</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0705514406226962</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0845181160231516</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.100697499706794</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1182932421922</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.137503102112429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.157450649420373</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.175422995320265</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.191261384593387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$C$30:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0317999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0403000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0372666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0338000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0325199999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0313333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0308571428571427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0303749999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0301333333333332</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0294799999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task3 - 2'!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision for overlapCaseSimilarity | MaxRecommender | dynamic directors &amp; dynamic genres &amp; static actors = 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$B$43:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0204792199688122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0602276980956696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0859343779444504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.100058126508605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.113695873915949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.128931231749876</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.141056377419401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.155378233962289</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16645955855214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.175956980684102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Task3 - 2'!$C$43:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0490000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0469333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0408999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0369599999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0348666666666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.032742857142857</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0313999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.029911111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0285799999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2105112320"/>
+        <c:axId val="-2115852368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2105112320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Recall</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2115852368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2115852368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Pr</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>écision</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2105112320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Precision =</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> f(Recall)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>Task1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1919,7 +2746,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2820,7 +3647,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -3851,6 +4678,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5400,6 +6267,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5969,6 +7352,43 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="10" name="Graphique 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
@@ -5987,7 +7407,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6024,7 +7444,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6324,10 +7744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:C52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6336,21 +7756,24 @@
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6358,10 +7781,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -6372,7 +7795,7 @@
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -6383,7 +7806,7 @@
         <v>4.6400000000000198E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -6394,7 +7817,7 @@
         <v>4.5733333333333598E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>20</v>
       </c>
@@ -6405,7 +7828,7 @@
         <v>4.0549999999999899E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>25</v>
       </c>
@@ -6416,7 +7839,7 @@
         <v>3.6439999999999598E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>30</v>
       </c>
@@ -6427,7 +7850,7 @@
         <v>3.4166666666666901E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>35</v>
       </c>
@@ -6438,7 +7861,7 @@
         <v>3.2114285714285602E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>40</v>
       </c>
@@ -6449,7 +7872,7 @@
         <v>2.9999999999999801E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>45</v>
       </c>
@@ -6460,7 +7883,7 @@
         <v>2.8644444444444299E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>50</v>
       </c>
@@ -6471,21 +7894,21 @@
         <v>2.7259999999999701E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -6632,10 +8055,10 @@
         <v>5</v>
       </c>
       <c r="B30">
-        <v>2.04061253993961E-2</v>
+        <v>6.2660812634109803E-3</v>
       </c>
       <c r="C30">
-        <v>3.1799999999999898E-2</v>
+        <v>1.19999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -6643,10 +8066,10 @@
         <v>10</v>
       </c>
       <c r="B31">
-        <v>5.1260627099903901E-2</v>
+        <v>1.4031638291160799E-2</v>
       </c>
       <c r="C31">
-        <v>4.0300000000000197E-2</v>
+        <v>1.44999999999999E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -6654,10 +8077,10 @@
         <v>15</v>
       </c>
       <c r="B32">
-        <v>7.0551440622696193E-2</v>
+        <v>1.94949970560057E-2</v>
       </c>
       <c r="C32">
-        <v>3.7266666666666698E-2</v>
+        <v>1.41999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -6665,10 +8088,10 @@
         <v>20</v>
       </c>
       <c r="B33">
-        <v>8.4518116023151596E-2</v>
+        <v>2.2994451541511401E-2</v>
       </c>
       <c r="C33">
-        <v>3.3800000000000101E-2</v>
+        <v>1.29E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -6676,10 +8099,10 @@
         <v>25</v>
       </c>
       <c r="B34">
-        <v>0.10069749970679399</v>
+        <v>2.8228225359431199E-2</v>
       </c>
       <c r="C34">
-        <v>3.2519999999999598E-2</v>
+        <v>1.2559999999999899E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -6687,10 +8110,10 @@
         <v>30</v>
       </c>
       <c r="B35">
-        <v>0.1182932421922</v>
+        <v>3.1705702120496997E-2</v>
       </c>
       <c r="C35">
-        <v>3.1333333333333602E-2</v>
+        <v>1.20333333333333E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -6698,10 +8121,10 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>0.137503102112429</v>
+        <v>3.41864219845113E-2</v>
       </c>
       <c r="C36">
-        <v>3.0857142857142701E-2</v>
+        <v>1.1342857142857101E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -6709,10 +8132,10 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>0.15745064942037301</v>
+        <v>3.8170743868827101E-2</v>
       </c>
       <c r="C37">
-        <v>3.0374999999999801E-2</v>
+        <v>1.1025E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -6720,10 +8143,10 @@
         <v>45</v>
       </c>
       <c r="B38">
-        <v>0.17542299532026501</v>
+        <v>4.4066162932927297E-2</v>
       </c>
       <c r="C38">
-        <v>3.01333333333332E-2</v>
+        <v>1.11555555555555E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -6731,15 +8154,10 @@
         <v>50</v>
       </c>
       <c r="B39">
-        <v>0.19126138459338701</v>
+        <v>4.6324508712125297E-2</v>
       </c>
       <c r="C39">
-        <v>2.94799999999996E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>2</v>
+        <v>1.05799999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -6762,110 +8180,50 @@
       <c r="A43">
         <v>5</v>
       </c>
-      <c r="B43">
-        <v>2.04792199688122E-2</v>
-      </c>
-      <c r="C43">
-        <v>3.9800000000000002E-2</v>
-      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>10</v>
       </c>
-      <c r="B44">
-        <v>6.02276980956696E-2</v>
-      </c>
-      <c r="C44">
-        <v>4.90000000000003E-2</v>
-      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>15</v>
       </c>
-      <c r="B45">
-        <v>8.5934377944450399E-2</v>
-      </c>
-      <c r="C45">
-        <v>4.6933333333333598E-2</v>
-      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>20</v>
       </c>
-      <c r="B46">
-        <v>0.100058126508605</v>
-      </c>
-      <c r="C46">
-        <v>4.0899999999999902E-2</v>
-      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>25</v>
       </c>
-      <c r="B47">
-        <v>0.113695873915949</v>
-      </c>
-      <c r="C47">
-        <v>3.6959999999999597E-2</v>
-      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>30</v>
       </c>
-      <c r="B48">
-        <v>0.128931231749876</v>
-      </c>
-      <c r="C48">
-        <v>3.48666666666669E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>35</v>
       </c>
-      <c r="B49">
-        <v>0.141056377419401</v>
-      </c>
-      <c r="C49">
-        <v>3.2742857142856997E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>40</v>
       </c>
-      <c r="B50">
-        <v>0.155378233962289</v>
-      </c>
-      <c r="C50">
-        <v>3.1399999999999803E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>45</v>
       </c>
-      <c r="B51">
-        <v>0.16645955855214001</v>
-      </c>
-      <c r="C51">
-        <v>2.9911111111111E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
-      </c>
-      <c r="B52">
-        <v>0.17595698068410201</v>
-      </c>
-      <c r="C52">
-        <v>2.8579999999999599E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6875,6 +8233,564 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.0380213582374501E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.6902059532952902E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6400000000000198E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.4398183555763701E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.5733333333333598E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.10084572353488799</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.0549999999999899E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.113159897522775</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.6439999999999598E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.126741910253064</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.4166666666666901E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.13848992915010699</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.2114285714285602E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.14650328830543499</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9999999999999801E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0.15635923079943401</v>
+      </c>
+      <c r="C12">
+        <v>2.8644444444444299E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>0.164044569093654</v>
+      </c>
+      <c r="C13">
+        <v>2.7259999999999701E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.5483433355763E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.27999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4.6237829322351903E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.45000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6.7523588274728694E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.4733333333333297E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.3531177534816606E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.26500000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9.7717955147187702E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.0959999999999599E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.113770434172071</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3.0133333333333599E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.127737352559784</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2.9057142857142702E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.137758668853834</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.7749999999999799E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>0.14514261073412699</v>
+      </c>
+      <c r="C25">
+        <v>2.6511111111110999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>0.15019709699067299</v>
+      </c>
+      <c r="C26">
+        <v>2.50799999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>2.04061253993961E-2</v>
+      </c>
+      <c r="C30">
+        <v>3.1799999999999898E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>5.1260627099903901E-2</v>
+      </c>
+      <c r="C31">
+        <v>4.0300000000000197E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>7.0551440622696193E-2</v>
+      </c>
+      <c r="C32">
+        <v>3.7266666666666698E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>8.4518116023151596E-2</v>
+      </c>
+      <c r="C33">
+        <v>3.3800000000000101E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>0.10069749970679399</v>
+      </c>
+      <c r="C34">
+        <v>3.2519999999999598E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.1182932421922</v>
+      </c>
+      <c r="C35">
+        <v>3.1333333333333602E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0.137503102112429</v>
+      </c>
+      <c r="C36">
+        <v>3.0857142857142701E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>0.15745064942037301</v>
+      </c>
+      <c r="C37">
+        <v>3.0374999999999801E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>0.17542299532026501</v>
+      </c>
+      <c r="C38">
+        <v>3.01333333333332E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>0.19126138459338701</v>
+      </c>
+      <c r="C39">
+        <v>2.94799999999996E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>2.04792199688122E-2</v>
+      </c>
+      <c r="C43">
+        <v>3.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>6.02276980956696E-2</v>
+      </c>
+      <c r="C44">
+        <v>4.90000000000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>8.5934377944450399E-2</v>
+      </c>
+      <c r="C45">
+        <v>4.6933333333333598E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>0.100058126508605</v>
+      </c>
+      <c r="C46">
+        <v>4.0899999999999902E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>0.113695873915949</v>
+      </c>
+      <c r="C47">
+        <v>3.6959999999999597E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>30</v>
+      </c>
+      <c r="B48">
+        <v>0.128931231749876</v>
+      </c>
+      <c r="C48">
+        <v>3.48666666666669E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>35</v>
+      </c>
+      <c r="B49">
+        <v>0.141056377419401</v>
+      </c>
+      <c r="C49">
+        <v>3.2742857142856997E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>40</v>
+      </c>
+      <c r="B50">
+        <v>0.155378233962289</v>
+      </c>
+      <c r="C50">
+        <v>3.1399999999999803E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>45</v>
+      </c>
+      <c r="B51">
+        <v>0.16645955855214001</v>
+      </c>
+      <c r="C51">
+        <v>2.9911111111111E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>0.17595698068410201</v>
+      </c>
+      <c r="C52">
+        <v>2.8579999999999599E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
@@ -7426,7 +9342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
@@ -8110,7 +10026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>

</xml_diff>